<commit_message>
Adicionando Itens ao orchestrador
</commit_message>
<xml_diff>
--- a/1RoboticEnterpriseFramework/Data/Config.xlsx
+++ b/1RoboticEnterpriseFramework/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PC\RPA Cours\M Cruz Uipath RPA REFRAME 2024\1RoboticEnterpriseFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B3A54E-CD59-40A6-ABFF-5997226D47E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89D2E9B-8263-48D7-8FC4-4C8B9A2CF117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -98,83 +98,82 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>ProcessToKill</t>
+  </si>
+  <si>
+    <t>chrome,EXCEL</t>
+  </si>
+  <si>
+    <t>AcmeSystem1_LoginPageUrl</t>
+  </si>
+  <si>
+    <t>AcmeSyste,1_Credenciais</t>
+  </si>
+  <si>
+    <t>AcmeSyste,1_WorkItensàgeUrl</t>
+  </si>
+  <si>
+    <t>AcmeSystem1_Witems</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
-    <t>ProcessToKill</t>
-  </si>
-  <si>
-    <t>chrome,EXCEL</t>
-  </si>
-  <si>
-    <t>AcmeSystem1_LoginPageUrl</t>
-  </si>
-  <si>
-    <t>AcmeSyste,1_Credenciais</t>
-  </si>
-  <si>
-    <t>AcmeSyste,1_WorkItensàgeUrl</t>
   </si>
 </sst>
 </file>
@@ -581,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -629,10 +628,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -640,11 +639,11 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -662,19 +661,19 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1731,18 +1730,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1766,7 +1765,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1788,7 +1787,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1799,7 +1798,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1810,53 +1809,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2840,7 +2839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2860,7 +2859,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2890,18 +2889,18 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>